<commit_message>
Changed from 13th Alley to 14th St
</commit_message>
<xml_diff>
--- a/templates/events/pdfs/Five_Rivers.xlsx
+++ b/templates/events/pdfs/Five_Rivers.xlsx
@@ -156,9 +156,6 @@
     <t xml:space="preserve"> Pearl St</t>
   </si>
   <si>
-    <t xml:space="preserve"> E 13th Alley</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Oak Alley</t>
   </si>
   <si>
@@ -394,6 +391,9 @@
   </si>
   <si>
     <t>Finish at Falling Sky Brewpub, Eugene.   Open 13:23, Close 21:00.</t>
+  </si>
+  <si>
+    <t>14th Ave</t>
   </si>
 </sst>
 </file>
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,16 +942,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>46</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="38" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
       <c r="B2" s="8"/>
       <c r="C2" s="15"/>
       <c r="D2" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -991,7 +991,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1036,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1066,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1078,10 +1078,10 @@
         <v>0.15999999999999992</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1121,7 +1121,7 @@
         <v>6.1</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>3</v>
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1181,10 +1181,10 @@
         <v>5.9999999999998721E-2</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1242,7 +1242,7 @@
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1287,7 +1287,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1299,10 +1299,10 @@
         <v>6.2999999999999972</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="38" x14ac:dyDescent="0.25">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1342,10 +1342,10 @@
         <v>4.25</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1360,22 +1360,22 @@
         <v>0</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F29" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="G29" s="18" t="s">
+      <c r="H29" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="H29" s="18" t="s">
-        <v>80</v>
-      </c>
       <c r="I29" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="J29" s="20" t="s">
         <v>94</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1388,10 +1388,10 @@
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G30" s="3">
         <v>0</v>
@@ -1415,13 +1415,13 @@
         <v>3.3599999999999923</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G31" s="3">
         <v>5.5</v>
@@ -1443,10 +1443,10 @@
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G32" s="3">
         <v>21.6</v>
@@ -1477,7 +1477,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G33" s="3">
         <v>62.3</v>
@@ -1504,7 +1504,7 @@
         <v>12</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G34" s="3">
         <v>72.5</v>
@@ -1531,7 +1531,7 @@
         <v>13</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G35" s="3">
         <v>82</v>
@@ -1562,7 +1562,7 @@
         <v>13</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G36" s="3">
         <v>126</v>
@@ -1589,7 +1589,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G37" s="26">
         <v>128.80000000000001</v>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1657,7 +1657,7 @@
         <v>2.9000000000000057</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>16</v>
@@ -1690,7 +1690,7 @@
         <v>4</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1705,7 +1705,7 @@
         <v>4</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1750,7 +1750,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="38" x14ac:dyDescent="0.25">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1775,10 +1775,10 @@
         <v>3.0000000000001137E-2</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1805,7 +1805,7 @@
         <v>2.3200000000000074</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>21</v>
@@ -1823,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
         <v>2.6299999999999955</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>22</v>
@@ -1898,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="38" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1926,7 +1926,7 @@
         <v>0</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1971,7 +1971,7 @@
         <v>0</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -1986,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2001,7 +2001,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2056,7 +2056,7 @@
         <v>0.51999999999999602</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>30</v>
@@ -2161,7 +2161,7 @@
         <v>0.50999999999999091</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D75" s="12" t="s">
         <v>37</v>
@@ -2179,7 +2179,7 @@
         <v>1</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2191,10 +2191,10 @@
         <v>1.3100000000000023</v>
       </c>
       <c r="C77" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D77" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="D77" s="12" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="38" x14ac:dyDescent="0.25">
@@ -2207,7 +2207,7 @@
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2249,10 +2249,10 @@
         <v>1.3200000000000074</v>
       </c>
       <c r="C81" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2267,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2282,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
         <v>1</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2327,7 +2327,7 @@
         <v>1</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2342,7 +2342,7 @@
         <v>1</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -2354,15 +2354,15 @@
         <v>2.0000000000010232E-2</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C90" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2370,7 +2370,7 @@
         <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2378,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2386,39 +2386,39 @@
         <v>4</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C94" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C95" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C96" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C97" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Event details for Lunch in Veneta, Feb 22.
</commit_message>
<xml_diff>
--- a/templates/events/pdfs/Five_Rivers.xlsx
+++ b/templates/events/pdfs/Five_Rivers.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michal/Dropbox/Sys/will-rando/templates/events/pdfs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA56CAD4-0313-4E4F-B9E3-10AEB3205DA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="460" windowWidth="20340" windowHeight="17460"/>
+    <workbookView xWindow="8460" yWindow="460" windowWidth="20340" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Five Rivers Cues" sheetId="1" r:id="rId1"/>
     <sheet name="x" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Five Rivers Cues'!$A$1:$D$97</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Five Rivers Cues'!$A$1:$E$97</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
   <si>
     <t>L</t>
   </si>
@@ -288,9 +289,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t xml:space="preserve">Info control: McKenzie View.  Answer question on card at intersection, then proceed right on McKenzie View. </t>
-  </si>
-  <si>
     <t>McKenzie View</t>
   </si>
   <si>
@@ -318,12 +316,6 @@
     <t>Close</t>
   </si>
   <si>
-    <t>Control: Walterville Market, just before Camp Creek ends at Mckenzie Highway. Open 08:32, Close 09:50.</t>
-  </si>
-  <si>
-    <t>Control: Lebanon Safeway.  Food, restrooms.  Open 11:23, Close 16:18.</t>
-  </si>
-  <si>
     <t>Street / notes</t>
   </si>
   <si>
@@ -369,9 +361,6 @@
     <t>Take path on right where available; passes under cross streets</t>
   </si>
   <si>
-    <t>Full City Coffee, 842 Pearl Street, Eugene OR.  Open 07:30, close 08:30.  Depart south (right) on Pearl, move left for turn.</t>
-  </si>
-  <si>
     <t>bc Cascade Dr  (after crossing Hwy 20/Santiam Hwy, SS)</t>
   </si>
   <si>
@@ -390,16 +379,34 @@
     <t xml:space="preserve"> High St (in front of Campbell Senior Center)</t>
   </si>
   <si>
-    <t>Finish at Falling Sky Brewpub, Eugene.   Open 13:23, Close 21:00.</t>
-  </si>
-  <si>
     <t>14th Ave</t>
+  </si>
+  <si>
+    <t>CTRL</t>
+  </si>
+  <si>
+    <t>Info control at end of McKenzie View Dr</t>
+  </si>
+  <si>
+    <t>Full City Coffee, 842 Pearl Street, Eugene OR.  Open 08:00, close 09:00.  Depart south (right) on Pearl, move left for turn.</t>
+  </si>
+  <si>
+    <t>Control: Dollar Geeral, just before Camp Creek ends at Mckenzie Highway. Open 09:02, Close 10:44.</t>
+  </si>
+  <si>
+    <t>Control: Lebanon Safeway.  Food, restrooms.  Open 11:53, Close 16:48.</t>
+  </si>
+  <si>
+    <t>Finish at Falling Sky Brewpub, Eugene.   Open 13:53, Close 21:30.</t>
+  </si>
+  <si>
+    <t>Cut</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -431,6 +438,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -438,6 +446,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -586,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -643,6 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,11 +932,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection sqref="A1:E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -934,13 +944,14 @@
     <col min="1" max="1" width="7.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="62.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="54.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
     <col min="7" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
@@ -951,20 +962,26 @@
         <v>45</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="38" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="40" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="15"/>
       <c r="D2" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="E2" s="32">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>0</v>
       </c>
@@ -978,8 +995,12 @@
       <c r="D3" s="11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E3" s="32">
+        <f>$E$2+(A3/9.6)/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>0.1</v>
       </c>
@@ -993,8 +1014,12 @@
       <c r="D4" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E4" s="32">
+        <f t="shared" ref="E4:E67" si="1">$E$2+(A4/9.6)/24</f>
+        <v>0.3337673611111111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>0.5</v>
       </c>
@@ -1008,8 +1033,12 @@
       <c r="D5" s="11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E5" s="32">
+        <f t="shared" si="1"/>
+        <v>0.33550347222222221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>0.7</v>
       </c>
@@ -1023,8 +1052,12 @@
       <c r="D6" s="11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E6" s="32">
+        <f t="shared" si="1"/>
+        <v>0.33637152777777773</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>1.4</v>
       </c>
@@ -1038,8 +1071,12 @@
       <c r="D7" s="11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E7" s="32">
+        <f t="shared" si="1"/>
+        <v>0.33940972222222221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>1.4</v>
       </c>
@@ -1053,8 +1090,12 @@
       <c r="D8" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E8" s="32">
+        <f t="shared" si="1"/>
+        <v>0.33940972222222221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>1.55</v>
       </c>
@@ -1066,10 +1107,14 @@
         <v>1</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="E9" s="32">
+        <f t="shared" si="1"/>
+        <v>0.3400607638888889</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>1.71</v>
       </c>
@@ -1083,8 +1128,12 @@
       <c r="D10" s="12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="38" x14ac:dyDescent="0.25">
+      <c r="E10" s="32">
+        <f t="shared" si="1"/>
+        <v>0.34075520833333334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>5.5</v>
       </c>
@@ -1092,32 +1141,42 @@
         <f t="shared" si="0"/>
         <v>3.79</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="C11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="32">
+        <f t="shared" si="1"/>
+        <v>0.3572048611111111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>5.5</v>
+        <v>11.6</v>
       </c>
       <c r="B12" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="32">
+        <f t="shared" si="1"/>
+        <v>0.38368055555555552</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>11.6</v>
       </c>
       <c r="B13" s="10">
-        <f t="shared" si="0"/>
+        <f>A13-A11</f>
         <v>6.1</v>
       </c>
       <c r="C13" s="15" t="s">
@@ -1126,8 +1185,12 @@
       <c r="D13" s="12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E13" s="32">
+        <f t="shared" si="1"/>
+        <v>0.38368055555555552</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>11.97</v>
       </c>
@@ -1141,8 +1204,12 @@
       <c r="D14" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E14" s="32">
+        <f t="shared" si="1"/>
+        <v>0.3852864583333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13.41</v>
       </c>
@@ -1156,8 +1223,12 @@
       <c r="D15" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="38" x14ac:dyDescent="0.25">
+      <c r="E15" s="32">
+        <f t="shared" si="1"/>
+        <v>0.39153645833333334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="40" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>21.64</v>
       </c>
@@ -1169,7 +1240,11 @@
         <v>1</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>95</v>
+        <v>119</v>
+      </c>
+      <c r="E16" s="32">
+        <f t="shared" si="1"/>
+        <v>0.42725694444444445</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1184,7 +1259,11 @@
         <v>50</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
+      </c>
+      <c r="E17" s="32">
+        <f t="shared" si="1"/>
+        <v>0.4275173611111111</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1201,6 +1280,10 @@
       <c r="D18" s="12" t="s">
         <v>7</v>
       </c>
+      <c r="E18" s="32">
+        <f t="shared" si="1"/>
+        <v>0.42782118055555551</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
@@ -1216,6 +1299,10 @@
       <c r="D19" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="E19" s="32">
+        <f t="shared" si="1"/>
+        <v>0.46358506944444444</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
@@ -1231,6 +1318,10 @@
       <c r="D20" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="E20" s="32">
+        <f t="shared" si="1"/>
+        <v>0.48828125</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="38" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
@@ -1244,6 +1335,10 @@
       <c r="D21" s="13" t="s">
         <v>53</v>
       </c>
+      <c r="E21" s="32">
+        <f t="shared" si="1"/>
+        <v>0.48875868055555555</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
@@ -1259,6 +1354,10 @@
       <c r="D22" s="11" t="s">
         <v>51</v>
       </c>
+      <c r="E22" s="32">
+        <f t="shared" si="1"/>
+        <v>0.48875868055555555</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
@@ -1274,6 +1373,10 @@
       <c r="D23" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="E23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.49539930555555556</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
@@ -1289,6 +1392,10 @@
       <c r="D24" s="12" t="s">
         <v>63</v>
       </c>
+      <c r="E24" s="32">
+        <f t="shared" si="1"/>
+        <v>0.54600694444444442</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
@@ -1304,6 +1411,10 @@
       <c r="D25" s="12" t="s">
         <v>52</v>
       </c>
+      <c r="E25" s="32">
+        <f t="shared" si="1"/>
+        <v>0.57335069444444442</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="38" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
@@ -1317,6 +1428,10 @@
       <c r="D26" s="13" t="s">
         <v>54</v>
       </c>
+      <c r="E26" s="32">
+        <f t="shared" si="1"/>
+        <v>0.57508680555555558</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
@@ -1332,6 +1447,10 @@
       <c r="D27" s="12" t="s">
         <v>9</v>
       </c>
+      <c r="E27" s="32">
+        <f t="shared" si="1"/>
+        <v>0.57625868055555551</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="38" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -1347,6 +1466,10 @@
       <c r="D28" s="12" t="s">
         <v>55</v>
       </c>
+      <c r="E28" s="32">
+        <f t="shared" si="1"/>
+        <v>0.59470486111111109</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
@@ -1362,6 +1485,10 @@
       <c r="D29" s="12" t="s">
         <v>56</v>
       </c>
+      <c r="E29" s="32">
+        <f t="shared" si="1"/>
+        <v>0.59600694444444446</v>
+      </c>
       <c r="F29" s="17" t="s">
         <v>77</v>
       </c>
@@ -1372,10 +1499,10 @@
         <v>79</v>
       </c>
       <c r="I29" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="J29" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1390,6 +1517,10 @@
       <c r="D30" s="9" t="s">
         <v>57</v>
       </c>
+      <c r="E30" s="32">
+        <f t="shared" si="1"/>
+        <v>0.60360243055555562</v>
+      </c>
       <c r="F30" s="21" t="s">
         <v>80</v>
       </c>
@@ -1420,8 +1551,12 @@
       <c r="D31" s="12" t="s">
         <v>10</v>
       </c>
+      <c r="E31" s="32">
+        <f t="shared" si="1"/>
+        <v>0.6181857638888888</v>
+      </c>
       <c r="F31" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G31" s="3">
         <v>5.5</v>
@@ -1445,6 +1580,10 @@
       <c r="D32" s="13" t="s">
         <v>62</v>
       </c>
+      <c r="E32" s="32">
+        <f t="shared" si="1"/>
+        <v>0.62174479166666674</v>
+      </c>
       <c r="F32" s="21" t="s">
         <v>81</v>
       </c>
@@ -1452,7 +1591,7 @@
         <v>21.6</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" ref="H32:H36" si="1">G32-G31</f>
+        <f t="shared" ref="H32:H36" si="2">G32-G31</f>
         <v>16.100000000000001</v>
       </c>
       <c r="I32" s="22">
@@ -1476,6 +1615,10 @@
       <c r="D33" s="12" t="s">
         <v>11</v>
       </c>
+      <c r="E33" s="32">
+        <f t="shared" si="1"/>
+        <v>0.62300347222222219</v>
+      </c>
       <c r="F33" s="21" t="s">
         <v>82</v>
       </c>
@@ -1483,7 +1626,7 @@
         <v>62.3</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40.699999999999996</v>
       </c>
       <c r="I33" s="3"/>
@@ -1503,14 +1646,18 @@
       <c r="D34" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="E34" s="32">
+        <f t="shared" si="1"/>
+        <v>0.62738715277777779</v>
+      </c>
       <c r="F34" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G34" s="3">
         <v>72.5</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10.200000000000003</v>
       </c>
       <c r="I34" s="3"/>
@@ -1530,6 +1677,10 @@
       <c r="D35" s="12" t="s">
         <v>13</v>
       </c>
+      <c r="E35" s="32">
+        <f t="shared" si="1"/>
+        <v>0.62738715277777779</v>
+      </c>
       <c r="F35" s="21" t="s">
         <v>83</v>
       </c>
@@ -1537,7 +1688,7 @@
         <v>82</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5</v>
       </c>
       <c r="I35" s="22">
@@ -1561,14 +1712,18 @@
       <c r="D36" s="12" t="s">
         <v>13</v>
       </c>
+      <c r="E36" s="32">
+        <f t="shared" si="1"/>
+        <v>0.62786458333333339</v>
+      </c>
       <c r="F36" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G36" s="3">
         <v>126</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="I36" s="3"/>
@@ -1588,6 +1743,10 @@
       <c r="D37" s="12" t="s">
         <v>14</v>
       </c>
+      <c r="E37" s="32">
+        <f t="shared" si="1"/>
+        <v>0.63116319444444446</v>
+      </c>
       <c r="F37" s="25" t="s">
         <v>84</v>
       </c>
@@ -1595,7 +1754,7 @@
         <v>128.80000000000001</v>
       </c>
       <c r="H37" s="26">
-        <f t="shared" ref="H37" si="2">G37-G36</f>
+        <f t="shared" ref="H37" si="3">G37-G36</f>
         <v>2.8000000000000114</v>
       </c>
       <c r="I37" s="27">
@@ -1619,6 +1778,10 @@
       <c r="D38" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="E38" s="32">
+        <f t="shared" si="1"/>
+        <v>0.63177083333333339</v>
+      </c>
     </row>
     <row r="39" spans="1:10" ht="38" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
@@ -1630,7 +1793,11 @@
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="E39" s="32">
+        <f t="shared" si="1"/>
+        <v>0.64800347222222221</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1647,6 +1814,10 @@
       <c r="D40" s="12" t="s">
         <v>15</v>
       </c>
+      <c r="E40" s="32">
+        <f t="shared" si="1"/>
+        <v>0.64809027777777772</v>
+      </c>
     </row>
     <row r="41" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
@@ -1662,6 +1833,10 @@
       <c r="D41" s="12" t="s">
         <v>16</v>
       </c>
+      <c r="E41" s="32">
+        <f t="shared" si="1"/>
+        <v>0.6606770833333333</v>
+      </c>
     </row>
     <row r="42" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
@@ -1677,6 +1852,10 @@
       <c r="D42" s="12" t="s">
         <v>17</v>
       </c>
+      <c r="E42" s="32">
+        <f t="shared" si="1"/>
+        <v>0.66471354166666663</v>
+      </c>
     </row>
     <row r="43" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
@@ -1690,7 +1869,11 @@
         <v>4</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
+      </c>
+      <c r="E43" s="32">
+        <f t="shared" si="1"/>
+        <v>0.67230902777777768</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1705,7 +1888,11 @@
         <v>4</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>114</v>
+        <v>110</v>
+      </c>
+      <c r="E44" s="32">
+        <f t="shared" si="1"/>
+        <v>0.68190104166666665</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1722,6 +1909,10 @@
       <c r="D45" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="E45" s="32">
+        <f t="shared" si="1"/>
+        <v>0.68467881944444442</v>
+      </c>
     </row>
     <row r="46" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
@@ -1737,6 +1928,10 @@
       <c r="D46" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="E46" s="32">
+        <f t="shared" si="1"/>
+        <v>0.68506944444444451</v>
+      </c>
     </row>
     <row r="47" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
@@ -1750,10 +1945,14 @@
         <v>1</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="38" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E47" s="32">
+        <f t="shared" si="1"/>
+        <v>0.68936631944444438</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="40" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>82</v>
       </c>
@@ -1763,10 +1962,14 @@
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="E48" s="32">
+        <f t="shared" si="1"/>
+        <v>0.68923611111111116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>82.03</v>
       </c>
@@ -1778,10 +1981,14 @@
         <v>50</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="E49" s="32">
+        <f t="shared" si="1"/>
+        <v>0.68936631944444438</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>82.66</v>
       </c>
@@ -1795,8 +2002,12 @@
       <c r="D50" s="12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E50" s="32">
+        <f t="shared" si="1"/>
+        <v>0.69210069444444444</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>84.98</v>
       </c>
@@ -1810,8 +2021,12 @@
       <c r="D51" s="12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E51" s="32">
+        <f t="shared" si="1"/>
+        <v>0.70217013888888891</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>86.75</v>
       </c>
@@ -1825,8 +2040,12 @@
       <c r="D52" s="12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E52" s="32">
+        <f t="shared" si="1"/>
+        <v>0.70985243055555558</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>89.38</v>
       </c>
@@ -1840,8 +2059,12 @@
       <c r="D53" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E53" s="32">
+        <f t="shared" si="1"/>
+        <v>0.72126736111111112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>94.14</v>
       </c>
@@ -1855,8 +2078,12 @@
       <c r="D54" s="12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E54" s="32">
+        <f t="shared" si="1"/>
+        <v>0.74192708333333335</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>94.62</v>
       </c>
@@ -1870,8 +2097,12 @@
       <c r="D55" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E55" s="32">
+        <f t="shared" si="1"/>
+        <v>0.74401041666666667</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>94.64</v>
       </c>
@@ -1885,8 +2116,12 @@
       <c r="D56" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E56" s="32">
+        <f t="shared" si="1"/>
+        <v>0.74409722222222219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>95.18</v>
       </c>
@@ -1900,8 +2135,12 @@
       <c r="D57" s="12" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="38" x14ac:dyDescent="0.25">
+      <c r="E57" s="32">
+        <f t="shared" si="1"/>
+        <v>0.74644097222222228</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="38" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>95.25</v>
       </c>
@@ -1913,8 +2152,12 @@
       <c r="D58" s="13" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E58" s="32">
+        <f t="shared" si="1"/>
+        <v>0.74674479166666663</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>95.25</v>
       </c>
@@ -1928,8 +2171,12 @@
       <c r="D59" s="12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E59" s="32">
+        <f t="shared" si="1"/>
+        <v>0.74674479166666663</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>103.31</v>
       </c>
@@ -1943,8 +2190,12 @@
       <c r="D60" s="12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E60" s="32">
+        <f t="shared" si="1"/>
+        <v>0.78172743055555549</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>106.08</v>
       </c>
@@ -1958,8 +2209,12 @@
       <c r="D61" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E61" s="32">
+        <f t="shared" si="1"/>
+        <v>0.79374999999999996</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>109.34</v>
       </c>
@@ -1973,8 +2228,12 @@
       <c r="D62" s="12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E62" s="32">
+        <f t="shared" si="1"/>
+        <v>0.80789930555555556</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>117.1</v>
       </c>
@@ -1988,8 +2247,12 @@
       <c r="D63" s="12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E63" s="32">
+        <f t="shared" si="1"/>
+        <v>0.84157986111111116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>117.31</v>
       </c>
@@ -2003,8 +2266,12 @@
       <c r="D64" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E64" s="32">
+        <f t="shared" si="1"/>
+        <v>0.84249131944444455</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>117.4</v>
       </c>
@@ -2016,13 +2283,17 @@
       <c r="D65" s="13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E65" s="32">
+        <f t="shared" si="1"/>
+        <v>0.84288194444444442</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>120</v>
       </c>
       <c r="B66" s="10">
-        <f t="shared" ref="B66:B88" si="3">A66-A65</f>
+        <f t="shared" ref="B66:B88" si="4">A66-A65</f>
         <v>2.5999999999999943</v>
       </c>
       <c r="C66" s="15" t="s">
@@ -2031,13 +2302,17 @@
       <c r="D66" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E66" s="32">
+        <f t="shared" si="1"/>
+        <v>0.85416666666666674</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>120.31</v>
       </c>
       <c r="B67" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.31000000000000227</v>
       </c>
       <c r="C67" s="15" t="s">
@@ -2046,13 +2321,17 @@
       <c r="D67" s="12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E67" s="32">
+        <f t="shared" si="1"/>
+        <v>0.85551215277777781</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>120.83</v>
       </c>
       <c r="B68" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.51999999999999602</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -2061,13 +2340,17 @@
       <c r="D68" s="12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E68" s="32">
+        <f t="shared" ref="E68:E87" si="5">$E$2+(A68/9.6)/24</f>
+        <v>0.85776909722222228</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>121.11</v>
       </c>
       <c r="B69" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.28000000000000114</v>
       </c>
       <c r="C69" s="15" t="s">
@@ -2076,13 +2359,17 @@
       <c r="D69" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E69" s="32">
+        <f t="shared" si="5"/>
+        <v>0.85898437499999991</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>121.48</v>
       </c>
       <c r="B70" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.37000000000000455</v>
       </c>
       <c r="C70" s="15" t="s">
@@ -2091,13 +2378,17 @@
       <c r="D70" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E70" s="32">
+        <f t="shared" si="5"/>
+        <v>0.86059027777777786</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>121.5</v>
       </c>
       <c r="B71" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9999999999996021E-2</v>
       </c>
       <c r="C71" s="15" t="s">
@@ -2106,13 +2397,17 @@
       <c r="D71" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E71" s="32">
+        <f t="shared" si="5"/>
+        <v>0.86067708333333326</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>121.59</v>
       </c>
       <c r="B72" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.0000000000003411E-2</v>
       </c>
       <c r="C72" s="15" t="s">
@@ -2121,13 +2416,17 @@
       <c r="D72" s="12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E72" s="32">
+        <f t="shared" si="5"/>
+        <v>0.86106770833333335</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>121.82</v>
       </c>
       <c r="B73" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.22999999999998977</v>
       </c>
       <c r="C73" s="15" t="s">
@@ -2136,13 +2435,17 @@
       <c r="D73" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E73" s="32">
+        <f t="shared" si="5"/>
+        <v>0.86206597222222214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>121.9</v>
       </c>
       <c r="B74" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.0000000000012506E-2</v>
       </c>
       <c r="C74" s="15" t="s">
@@ -2151,13 +2454,17 @@
       <c r="D74" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E74" s="32">
+        <f t="shared" si="5"/>
+        <v>0.86241319444444442</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>122.41</v>
       </c>
       <c r="B75" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.50999999999999091</v>
       </c>
       <c r="C75" s="15" t="s">
@@ -2166,38 +2473,50 @@
       <c r="D75" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E75" s="32">
+        <f t="shared" si="5"/>
+        <v>0.86462673611111107</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>123.09</v>
       </c>
       <c r="B76" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.68000000000000682</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="E76" s="32">
+        <f t="shared" si="5"/>
+        <v>0.86757812500000009</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>124.4</v>
       </c>
       <c r="B77" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3100000000000023</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="38" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="E77" s="32">
+        <f t="shared" si="5"/>
+        <v>0.87326388888888884</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="38" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>126</v>
       </c>
@@ -2207,15 +2526,19 @@
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="E78" s="32">
+        <f t="shared" si="5"/>
+        <v>0.88020833333333326</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>126.01</v>
       </c>
       <c r="B79" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0000000000005116E-2</v>
       </c>
       <c r="C79" s="15" t="s">
@@ -2224,13 +2547,17 @@
       <c r="D79" s="12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E79" s="32">
+        <f t="shared" si="5"/>
+        <v>0.88025173611111107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>126.13</v>
       </c>
       <c r="B80" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.11999999999999034</v>
       </c>
       <c r="C80" s="15" t="s">
@@ -2239,13 +2566,17 @@
       <c r="D80" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E80" s="32">
+        <f t="shared" si="5"/>
+        <v>0.88077256944444438</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>127.45</v>
       </c>
       <c r="B81" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3200000000000074</v>
       </c>
       <c r="C81" s="15" t="s">
@@ -2254,43 +2585,55 @@
       <c r="D81" s="12" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E81" s="32">
+        <f t="shared" si="5"/>
+        <v>0.88650173611111116</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>127.62</v>
       </c>
       <c r="B82" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.17000000000000171</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="E82" s="32">
+        <f t="shared" si="5"/>
+        <v>0.8872395833333333</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>127.68</v>
       </c>
       <c r="B83" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.0000000000002274E-2</v>
       </c>
       <c r="C83" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="E83" s="32">
+        <f t="shared" si="5"/>
+        <v>0.88749999999999996</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>127.88</v>
       </c>
       <c r="B84" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.19999999999998863</v>
       </c>
       <c r="C84" s="15" t="s">
@@ -2299,13 +2642,17 @@
       <c r="D84" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E84" s="32">
+        <f t="shared" si="5"/>
+        <v>0.88836805555555554</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>127.96</v>
       </c>
       <c r="B85" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.9999999999998295E-2</v>
       </c>
       <c r="C85" s="15" t="s">
@@ -2314,28 +2661,36 @@
       <c r="D85" s="12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E85" s="32">
+        <f t="shared" si="5"/>
+        <v>0.88871527777777781</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>128.68</v>
       </c>
       <c r="B86" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.72000000000001307</v>
       </c>
       <c r="C86" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="E86" s="32">
+        <f t="shared" si="5"/>
+        <v>0.89184027777777786</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>128.79</v>
       </c>
       <c r="B87" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.10999999999998522</v>
       </c>
       <c r="C87" s="15" t="s">
@@ -2344,87 +2699,91 @@
       <c r="D87" s="12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="E87" s="32">
+        <f t="shared" si="5"/>
+        <v>0.89231770833333335</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="40" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>128.81</v>
       </c>
       <c r="B88" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.0000000000010232E-2</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>42</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C90" s="29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C91" s="30" t="s">
         <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C92" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C93" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C94" s="30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C95" s="30" t="s">
         <v>50</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C96" s="30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C97" s="31" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri (Body),Regular"&amp;22Five Rivers Brevet (Eugene, OR)</oddHeader>
   </headerFooter>
@@ -2437,7 +2796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>